<commit_message>
Updated various sprint deliverables in Documents folder.
</commit_message>
<xml_diff>
--- a/Documents/User Stories/Sprint 1 User Stories.xlsx
+++ b/Documents/User Stories/Sprint 1 User Stories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shady\Desktop\grad_school_stuff\class\cs691 capstone\sprint 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shady\Desktop\grad_school_stuff\class\cs691 capstone\repo\integ_merge\Documents\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E543C02-DDB8-4E33-B317-DBDC1FDDF9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5686241-6D82-45ED-A603-C582B1CB7320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30120" yWindow="1500" windowWidth="26760" windowHeight="13065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6615" yWindow="1785" windowWidth="21765" windowHeight="13455" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1350,10 +1350,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3107B872-F0A2-43CD-A027-7B6FAED7AA11}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,7 +1642,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>